<commit_message>
Improved PAA questions and answers.
</commit_message>
<xml_diff>
--- a/scripts/keywords.xlsx
+++ b/scripts/keywords.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/konradburchardt/Desktop/People Also Ask/scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/konradburchardt/Desktop/Web development projects/SEO/People Also Ask/scripts/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB9CA6AA-FD43-3344-A21D-015B484BB3AC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44DC839-76A9-6D47-A3E3-135CBF5B2857}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2780" yWindow="1560" windowWidth="28040" windowHeight="17440" xr2:uid="{2345F025-E333-B34C-B596-6A1DC1302AAB}"/>
   </bookViews>
@@ -33,42 +33,34 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>Keywords</t>
   </si>
   <si>
-    <t>Netflix</t>
-  </si>
-  <si>
-    <t>Netflix stock</t>
-  </si>
-  <si>
-    <t>Netflix plan</t>
+    <t>Netflix Stock</t>
+  </si>
+  <si>
+    <t>Uber Stock</t>
+  </si>
+  <si>
+    <t>Disney Stock</t>
+  </si>
+  <si>
+    <t>Facebook Stock</t>
+  </si>
+  <si>
+    <t>Tesla Stock</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -91,17 +83,13 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -414,288 +402,46 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF5BC6EA-D1F4-6848-ACF4-2272578CB2EE}">
-  <dimension ref="A1:A88"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:A27"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
   <cols>
     <col min="1" max="1" width="18.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:1">
+      <c r="A3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
+    <row r="4" spans="1:1">
+      <c r="A4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A5" s="1"/>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A6" s="1"/>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A7" s="1"/>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A8" s="1"/>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A9" s="1"/>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A10" s="2"/>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A11" s="1"/>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A12" s="1"/>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A13" s="1"/>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A14" s="1"/>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A15" s="1"/>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A16" s="1"/>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A17" s="1"/>
-    </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A18" s="1"/>
-    </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A19" s="1"/>
-    </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A20" s="1"/>
-    </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A21" s="1"/>
-    </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A22" s="1"/>
-    </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A23" s="1"/>
-    </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A24" s="1"/>
-    </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A25" s="1"/>
-    </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A26" s="1"/>
-    </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A27" s="1"/>
-    </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A28" s="1"/>
-    </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A29" s="1"/>
-    </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A30" s="1"/>
-    </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A31" s="1"/>
-    </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A32" s="1"/>
-    </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A33" s="1"/>
-    </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A34" s="1"/>
-    </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A35" s="1"/>
-    </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A36" s="1"/>
-    </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A37" s="1"/>
-    </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A38" s="1"/>
-    </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A39" s="1"/>
-    </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A40" s="1"/>
-    </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A41" s="1"/>
-    </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A42" s="1"/>
-    </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A43" s="1"/>
-    </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A44" s="1"/>
-    </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A45" s="1"/>
-    </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A46" s="1"/>
-    </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A47" s="1"/>
-    </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A48" s="1"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="1"/>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="1"/>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="1"/>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="1"/>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" s="1"/>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" s="1"/>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" s="1"/>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" s="1"/>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" s="1"/>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" s="1"/>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" s="1"/>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A60" s="1"/>
-    </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A61" s="1"/>
-    </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A62" s="1"/>
-    </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A63" s="1"/>
-    </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A64" s="1"/>
-    </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A65" s="1"/>
-    </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A66" s="1"/>
-    </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A67" s="1"/>
-    </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A68" s="1"/>
-    </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A69" s="1"/>
-    </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A70" s="1"/>
-    </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A71" s="1"/>
-    </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A72" s="1"/>
-    </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A73" s="1"/>
-    </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A74" s="1"/>
-    </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A75" s="1"/>
-    </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A76" s="1"/>
-    </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A77" s="1"/>
-    </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A78" s="1"/>
-    </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A79" s="1"/>
-    </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A80" s="1"/>
-    </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A81" s="1"/>
-    </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A82" s="1"/>
-    </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A83" s="1"/>
-    </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A84" s="1"/>
-    </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A85" s="1"/>
-    </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A86" s="1"/>
-    </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A87" s="1"/>
-    </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A88" s="1"/>
+    <row r="5" spans="1:1">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" t="s">
+        <v>5</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>